<commit_message>
Add Cli command for players
</commit_message>
<xml_diff>
--- a/VereinsDaten.xlsx
+++ b/VereinsDaten.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>team_name</t>
   </si>
@@ -22,10 +22,16 @@
     <t>team_trainer</t>
   </si>
   <si>
+    <t>team_logo</t>
+  </si>
+  <si>
     <t>Hells Teddies</t>
   </si>
   <si>
     <t>test trainer</t>
+  </si>
+  <si>
+    <t>/Team-logos/logo1.png</t>
   </si>
   <si>
     <t>PPL</t>
@@ -313,7 +319,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -339,23 +347,29 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3">
         <v>2013.0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>2018.0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>